<commit_message>
added overtime by ilyas
</commit_message>
<xml_diff>
--- a/Табель за Август - г.Алматы.xlsx
+++ b/Табель за Август - г.Алматы.xlsx
@@ -483,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,40 +492,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="5" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="12" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="12" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="12" customWidth="1" min="21" max="21"/>
-    <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="12" customWidth="1" min="23" max="23"/>
-    <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="12" customWidth="1" min="25" max="25"/>
-    <col width="12" customWidth="1" min="26" max="26"/>
-    <col width="12" customWidth="1" min="27" max="27"/>
-    <col width="12" customWidth="1" min="28" max="28"/>
-    <col width="12" customWidth="1" min="29" max="29"/>
-    <col width="12" customWidth="1" min="30" max="30"/>
-    <col width="12" customWidth="1" min="31" max="31"/>
-    <col width="12" customWidth="1" min="32" max="32"/>
-    <col width="12" customWidth="1" min="33" max="33"/>
-    <col width="12" customWidth="1" min="34" max="34"/>
-    <col width="13" customWidth="1" min="35" max="35"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="7" max="7"/>
+    <col width="26" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="12" max="12"/>
+    <col width="22" customWidth="1" min="13" max="13"/>
+    <col width="26" customWidth="1" min="14" max="14"/>
+    <col width="26" customWidth="1" min="15" max="15"/>
+    <col width="22" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+    <col width="22" customWidth="1" min="19" max="19"/>
+    <col width="22" customWidth="1" min="20" max="20"/>
+    <col width="26" customWidth="1" min="21" max="21"/>
+    <col width="26" customWidth="1" min="22" max="22"/>
+    <col width="22" customWidth="1" min="23" max="23"/>
+    <col width="20" customWidth="1" min="24" max="24"/>
+    <col width="22" customWidth="1" min="25" max="25"/>
+    <col width="22" customWidth="1" min="26" max="26"/>
+    <col width="22" customWidth="1" min="27" max="27"/>
+    <col width="26" customWidth="1" min="28" max="28"/>
+    <col width="26" customWidth="1" min="29" max="29"/>
+    <col width="22" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="31" max="31"/>
+    <col width="22" customWidth="1" min="32" max="32"/>
+    <col width="22" customWidth="1" min="33" max="33"/>
+    <col width="22" customWidth="1" min="34" max="34"/>
+    <col width="17" customWidth="1" min="35" max="35"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -587,169 +587,169 @@
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-01 (Четверг)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-02</t>
+          <t>2024-08-02 (Пятница)</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-03</t>
+          <t>2024-08-03 (Суббота)</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-04</t>
+          <t>2024-08-04 (Воскресенье)</t>
         </is>
       </c>
       <c r="H2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-05</t>
+          <t>2024-08-05 (Понедельник)</t>
         </is>
       </c>
       <c r="I2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-06</t>
+          <t>2024-08-06 (Вторник)</t>
         </is>
       </c>
       <c r="J2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-07 (Среда)</t>
         </is>
       </c>
       <c r="K2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-08</t>
+          <t>2024-08-08 (Четверг)</t>
         </is>
       </c>
       <c r="L2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-09</t>
+          <t>2024-08-09 (Пятница)</t>
         </is>
       </c>
       <c r="M2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-10</t>
+          <t>2024-08-10 (Суббота)</t>
         </is>
       </c>
       <c r="N2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-11</t>
+          <t>2024-08-11 (Воскресенье)</t>
         </is>
       </c>
       <c r="O2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-12</t>
+          <t>2024-08-12 (Понедельник)</t>
         </is>
       </c>
       <c r="P2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-13</t>
+          <t>2024-08-13 (Вторник)</t>
         </is>
       </c>
       <c r="Q2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-14</t>
+          <t>2024-08-14 (Среда)</t>
         </is>
       </c>
       <c r="R2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-15</t>
+          <t>2024-08-15 (Четверг)</t>
         </is>
       </c>
       <c r="S2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-16</t>
+          <t>2024-08-16 (Пятница)</t>
         </is>
       </c>
       <c r="T2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-17</t>
+          <t>2024-08-17 (Суббота)</t>
         </is>
       </c>
       <c r="U2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-18</t>
+          <t>2024-08-18 (Воскресенье)</t>
         </is>
       </c>
       <c r="V2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-19</t>
+          <t>2024-08-19 (Понедельник)</t>
         </is>
       </c>
       <c r="W2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-20</t>
+          <t>2024-08-20 (Вторник)</t>
         </is>
       </c>
       <c r="X2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-08-21 (Среда)</t>
         </is>
       </c>
       <c r="Y2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-22</t>
+          <t>2024-08-22 (Четверг)</t>
         </is>
       </c>
       <c r="Z2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-23</t>
+          <t>2024-08-23 (Пятница)</t>
         </is>
       </c>
       <c r="AA2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-24</t>
+          <t>2024-08-24 (Суббота)</t>
         </is>
       </c>
       <c r="AB2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-25</t>
+          <t>2024-08-25 (Воскресенье)</t>
         </is>
       </c>
       <c r="AC2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-26</t>
+          <t>2024-08-26 (Понедельник)</t>
         </is>
       </c>
       <c r="AD2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-27</t>
+          <t>2024-08-27 (Вторник)</t>
         </is>
       </c>
       <c r="AE2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-28</t>
+          <t>2024-08-28 (Среда)</t>
         </is>
       </c>
       <c r="AF2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-29</t>
+          <t>2024-08-29 (Четверг)</t>
         </is>
       </c>
       <c r="AG2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-30</t>
+          <t>2024-08-30 (Пятница)</t>
         </is>
       </c>
       <c r="AH2" s="4" t="inlineStr">
         <is>
-          <t>2024-08-31</t>
+          <t>2024-08-31 (Суббота)</t>
         </is>
       </c>
       <c r="AI2" s="4" t="inlineStr">
         <is>
-          <t>Переработка</t>
+          <t>Переработка (ч)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -799,7 +799,7 @@
       <c r="AH3" s="3" t="inlineStr"/>
       <c r="AI3" s="3" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>00:00</t>
         </is>
       </c>
     </row>
@@ -1013,12 +1013,282 @@
       </c>
       <c r="AI5" s="6" t="n"/>
     </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>ilyas</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Время прихода</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr"/>
+      <c r="E6" s="3" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" s="3" t="inlineStr"/>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" s="3" t="inlineStr"/>
+      <c r="L6" s="3" t="inlineStr"/>
+      <c r="M6" s="3" t="inlineStr"/>
+      <c r="N6" s="3" t="inlineStr"/>
+      <c r="O6" s="3" t="inlineStr"/>
+      <c r="P6" s="3" t="inlineStr"/>
+      <c r="Q6" s="3" t="inlineStr"/>
+      <c r="R6" s="3" t="inlineStr"/>
+      <c r="S6" s="3" t="inlineStr"/>
+      <c r="T6" s="3" t="inlineStr"/>
+      <c r="U6" s="3" t="inlineStr"/>
+      <c r="V6" s="3" t="inlineStr"/>
+      <c r="W6" s="3" t="inlineStr"/>
+      <c r="X6" s="3" t="inlineStr"/>
+      <c r="Y6" s="3" t="inlineStr"/>
+      <c r="Z6" s="3" t="inlineStr"/>
+      <c r="AA6" s="3" t="inlineStr"/>
+      <c r="AB6" s="3" t="inlineStr">
+        <is>
+          <t>01:57</t>
+        </is>
+      </c>
+      <c r="AC6" s="3" t="inlineStr"/>
+      <c r="AD6" s="3" t="inlineStr"/>
+      <c r="AE6" s="3" t="inlineStr"/>
+      <c r="AF6" s="3" t="inlineStr"/>
+      <c r="AG6" s="3" t="inlineStr"/>
+      <c r="AH6" s="3" t="inlineStr"/>
+      <c r="AI6" s="3" t="inlineStr">
+        <is>
+          <t>09:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Время ухода</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr"/>
+      <c r="E7" s="3" t="inlineStr"/>
+      <c r="F7" s="3" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
+      <c r="I7" s="3" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" s="3" t="inlineStr"/>
+      <c r="L7" s="3" t="inlineStr"/>
+      <c r="M7" s="3" t="inlineStr"/>
+      <c r="N7" s="3" t="inlineStr"/>
+      <c r="O7" s="3" t="inlineStr"/>
+      <c r="P7" s="3" t="inlineStr"/>
+      <c r="Q7" s="3" t="inlineStr"/>
+      <c r="R7" s="3" t="inlineStr"/>
+      <c r="S7" s="3" t="inlineStr"/>
+      <c r="T7" s="3" t="inlineStr"/>
+      <c r="U7" s="3" t="inlineStr"/>
+      <c r="V7" s="3" t="inlineStr"/>
+      <c r="W7" s="3" t="inlineStr"/>
+      <c r="X7" s="3" t="inlineStr"/>
+      <c r="Y7" s="3" t="inlineStr"/>
+      <c r="Z7" s="3" t="inlineStr"/>
+      <c r="AA7" s="3" t="inlineStr"/>
+      <c r="AB7" s="3" t="inlineStr">
+        <is>
+          <t>11:46</t>
+        </is>
+      </c>
+      <c r="AC7" s="3" t="inlineStr"/>
+      <c r="AD7" s="3" t="inlineStr"/>
+      <c r="AE7" s="3" t="inlineStr"/>
+      <c r="AF7" s="3" t="inlineStr"/>
+      <c r="AG7" s="3" t="inlineStr"/>
+      <c r="AH7" s="3" t="inlineStr"/>
+      <c r="AI7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Кол-во часов</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="R8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="S8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="T8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="U8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="V8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="W8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="X8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="Y8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="Z8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AA8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AB8" s="3" t="inlineStr">
+        <is>
+          <t>09:49</t>
+        </is>
+      </c>
+      <c r="AC8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AD8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AE8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AF8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AG8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AH8" s="3" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="AI8" s="6" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="AI3:AI5"/>
+    <mergeCell ref="AI6:AI8"/>
     <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>